<commit_message>
Make sure the code works with the latest code table spreadsheets. Use DaoUtils.getInteger() instead of rs.getInt() to be able to get null instead of 0 when the column is indeed null.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/AdamsCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/AdamsCountyAnalyticsCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="28340" windowHeight="16060" tabRatio="951" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28340" windowHeight="16060" tabRatio="951" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -18,16 +18,15 @@
     <sheet name="JurisdictionType" sheetId="2" r:id="rId9"/>
     <sheet name="LanguageType" sheetId="15" r:id="rId10"/>
     <sheet name="MedicaidStatusType" sheetId="32" r:id="rId11"/>
-    <sheet name="MedicationType" sheetId="21" r:id="rId12"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId13"/>
-    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId14"/>
-    <sheet name="PersonRaceType" sheetId="7" r:id="rId15"/>
-    <sheet name="PersonSexType" sheetId="6" r:id="rId16"/>
-    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId17"/>
-    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId18"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId19"/>
-    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId20"/>
-    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId21"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId12"/>
+    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId13"/>
+    <sheet name="PersonRaceType" sheetId="7" r:id="rId14"/>
+    <sheet name="PersonSexType" sheetId="6" r:id="rId15"/>
+    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId16"/>
+    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId17"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId18"/>
+    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId19"/>
+    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="765">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -2235,15 +2234,6 @@
   </si>
   <si>
     <t>MedicaidStatusTypeDescription</t>
-  </si>
-  <si>
-    <t>MedicationTypeID</t>
-  </si>
-  <si>
-    <t>GenericProductIdentification</t>
-  </si>
-  <si>
-    <t>MedicationTypeDescription</t>
   </si>
   <si>
     <t>MilitaryServiceStatusTypeID</t>
@@ -2349,7 +2339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2375,6 +2365,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2477,9 +2474,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2995,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C2" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3006,10 +3004,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C3" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3078,45 +3076,6 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>732</v>
-      </c>
-      <c r="B1" t="s">
-        <v>733</v>
-      </c>
-      <c r="C1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3131,10 +3090,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="B1" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3236,7 +3195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3252,10 +3211,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B1" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3302,7 +3261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3319,10 +3278,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="B1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3402,7 +3361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3419,10 +3378,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="B1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3469,7 +3428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3513,7 +3472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3529,10 +3488,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="B1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3540,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3548,7 +3507,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3556,6 +3515,50 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3578,21 +3581,21 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="B1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3605,7 +3608,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3631,10 +3633,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="B1" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -6839,49 +6841,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>745</v>
-      </c>
-      <c r="B1" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -6908,7 +6867,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6916,7 +6875,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6990,10 +6949,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -7100,7 +7059,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C11" t="s">
         <v>120</v>
@@ -7111,7 +7070,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="C12" t="s">
         <v>119</v>
@@ -7693,7 +7652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -7716,7 +7675,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C2" t="s">
         <v>144</v>
@@ -7727,7 +7686,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C3" t="s">
         <v>143</v>
@@ -7738,7 +7697,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -7749,10 +7708,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C5" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -7822,10 +7781,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7843,10 +7802,1130 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="2">
+        <v>99999</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>